<commit_message>
Update app version to 1.1.7 and improve file generation script
</commit_message>
<xml_diff>
--- a/assets/files/samples/business_korean.xlsx
+++ b/assets/files/samples/business_korean.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -650,9 +650,169 @@
         <v>Keep up the good work. (Formal greeting)</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>자료 준비되었습니다.</v>
+      </c>
+      <c r="B32" t="str">
+        <v>The materials are ready.</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>언제 시간 되시나요?</v>
+      </c>
+      <c r="B33" t="str">
+        <v>When are you available?</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>점심 식사 하셨습니까?</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Have you had lunch?</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>커피 한 잔 하시겠습니까?</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Would you like a cup of coffee?</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>잠시 자리 비우셨습니다.</v>
+      </c>
+      <c r="B36" t="str">
+        <v>He/She is away from the desk for a moment.</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>메모 남겨드릴까요?</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Shall I leave a message?</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>팩스로 보내주세요.</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Please send it by fax.</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>프레젠테이션 준비 완료했습니다.</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Presentation preparation is complete.</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>예산안 검토 부탁드립니다.</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Please review the budget proposal.</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>다음 주 일정 잡겠습니다.</v>
+      </c>
+      <c r="B41" t="str">
+        <v>I will schedule it for next week.</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>출근했습니다.</v>
+      </c>
+      <c r="B42" t="str">
+        <v>I have arrived at work.</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>병가 내겠습니다.</v>
+      </c>
+      <c r="B43" t="str">
+        <v>I will take a sick leave.</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>연차 쓰겠습니다.</v>
+      </c>
+      <c r="B44" t="str">
+        <v>I will use my annual leave.</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>급한 일입니까?</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Is it urgent?</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>우선순위가 어떻게 되나요?</v>
+      </c>
+      <c r="B46" t="str">
+        <v>What is the priority?</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>피드백 부탁드립니다.</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Please give me feedback.</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>수정해서 다시 보내겠습니다.</v>
+      </c>
+      <c r="B48" t="str">
+        <v>I will revise and resend it.</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>성공적인 프로젝트였습니다.</v>
+      </c>
+      <c r="B49" t="str">
+        <v>It was a successful project.</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>함께 일해서 즐거웠습니다.</v>
+      </c>
+      <c r="B50" t="str">
+        <v>It was a pleasure working with you.</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>앞으로도 잘 부탁드립니다.</v>
+      </c>
+      <c r="B51" t="str">
+        <v>I look forward to working with you.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B51"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expand sample excel scripts to 100 sentences each using chunked approach
</commit_message>
<xml_diff>
--- a/assets/files/samples/business_korean.xlsx
+++ b/assets/files/samples/business_korean.xlsx
@@ -412,90 +412,90 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>안녕하세요. 이메일 잘 받았습니다.</v>
+        <v>안녕하십니까.</v>
       </c>
       <c r="B2" t="str">
-        <v>Hello. I received your email.</v>
+        <v>Greetings (Formal).</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>회의 일정은 언제인가요?</v>
+        <v>수고하셨습니다.</v>
       </c>
       <c r="B3" t="str">
-        <v>When is the meeting schedule?</v>
+        <v>Good job today. / Thank you for your effort.</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>보고서는 내일까지 제출해주세요.</v>
+        <v>회의 시작하겠습니다.</v>
       </c>
       <c r="B4" t="str">
-        <v>Please submit the report by tomorrow.</v>
+        <v>Let's start the meeting.</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>결재를 부탁드립니다.</v>
+        <v>의견 있으신가요?</v>
       </c>
       <c r="B5" t="str">
-        <v>Please approve this.</v>
+        <v>Do you have any opinions?</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>이번 프로젝트의 목표는 무엇인가요?</v>
+        <v>결재 부탁드립니다.</v>
       </c>
       <c r="B6" t="str">
-        <v>What is the goal of this project?</v>
+        <v>Please approve this.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>예산안을 검토해주세요.</v>
+        <v>보고서 제출했습니다.</v>
       </c>
       <c r="B7" t="str">
-        <v>Please review the budget proposal.</v>
+        <v>I submitted the report.</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>다음 주 출장 예정입니다.</v>
+        <v>이메일 확인 부탁드립니다.</v>
       </c>
       <c r="B8" t="str">
-        <v>I am scheduled for a business trip next week.</v>
+        <v>Please check your email.</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>회의실 예약했습니다.</v>
+        <v>오늘 회식 있나요?</v>
       </c>
       <c r="B9" t="str">
-        <v>I booked a meeting room.</v>
+        <v>Do we have a team dinner today?</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>잠시 통화 가능하신가요?</v>
+        <v>야근해야 할 것 같습니다.</v>
       </c>
       <c r="B10" t="str">
-        <v>Are you available for a call?</v>
+        <v>I think I have to work overtime.</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>지금은 회의 중입니다.</v>
+        <v>출장 다녀오겠습니다.</v>
       </c>
       <c r="B11" t="str">
-        <v>I am in a meeting right now.</v>
+        <v>I will go on a business trip.</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>나중에 다시 연락드리겠습니다.</v>
+        <v>죄송하지만, 잠시 통화 가능하신가요?</v>
       </c>
       <c r="B12" t="str">
-        <v>I will contact you later.</v>
+        <v>Sorry, can you talk for a moment?</v>
       </c>
     </row>
     <row r="13">
@@ -508,706 +508,706 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>협조해주셔서 감사합니다.</v>
+        <v>일정 확인해보겠습니다.</v>
       </c>
       <c r="B14" t="str">
-        <v>Thank you for your cooperation.</v>
+        <v>I will check the schedule.</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>문의사항이 있으시면 연락주세요.</v>
+        <v>협조해주셔서 감사합니다.</v>
       </c>
       <c r="B15" t="str">
-        <v>Please contact me if you have any questions.</v>
+        <v>Thank you for your cooperation.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>첨부 파일을 확인해주세요.</v>
+        <v>마감 기한은 언제인가요?</v>
       </c>
       <c r="B16" t="str">
-        <v>Please check the attached file.</v>
+        <v>When is the deadline?</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>빠른 회신 부탁드립니다.</v>
+        <v>문제 없습니다.</v>
       </c>
       <c r="B17" t="str">
-        <v>Please reply as soon as possible.</v>
+        <v>No problem.</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>거래처 미팅이 잡혔습니다.</v>
+        <v>검토 후 연락드리겠습니다.</v>
       </c>
       <c r="B18" t="str">
-        <v>A meeting with the client is scheduled.</v>
+        <v>I will contact you after review.</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>계약서 초안을 보냈습니다.</v>
+        <v>명함 한 장 주시겠습니까?</v>
       </c>
       <c r="B19" t="str">
-        <v>I sent the draft of the contract.</v>
+        <v>Could you give me your business card?</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>수정 사항이 있습니다.</v>
+        <v>승진 축하드립니다.</v>
       </c>
       <c r="B20" t="str">
-        <v>There are some revisions.</v>
+        <v>Congratulations on your promotion.</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>승인되었습니다.</v>
+        <v>휴가 잘 다녀오세요.</v>
       </c>
       <c r="B21" t="str">
-        <v>It has been approved.</v>
+        <v>Have a nice vacation.</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>반려되었습니다.</v>
+        <v>퇴근하겠습니다.</v>
       </c>
       <c r="B22" t="str">
-        <v>It has been rejected.</v>
+        <v>I'm leaving work now.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>추가 정보가 필요합니다.</v>
+        <v>내일 뵙겠습니다.</v>
       </c>
       <c r="B23" t="str">
-        <v>More information is needed.</v>
+        <v>See you tomorrow.</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>일정을 변경해야 할 것 같습니다.</v>
+        <v>양해 부탁드립니다.</v>
       </c>
       <c r="B24" t="str">
-        <v>I think we need to reschedule.</v>
+        <v>I ask for your understanding.</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>마감 기한을 지켜주세요.</v>
+        <v>최선을 다하겠습니다.</v>
       </c>
       <c r="B25" t="str">
-        <v>Please meet the deadline.</v>
+        <v>I will do my best.</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>진행 상황을 공유해주세요.</v>
+        <v>좋은 결과 기대하겠습니다.</v>
       </c>
       <c r="B26" t="str">
-        <v>Please share the progress.</v>
+        <v>I look forward to good results.</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>문제가 발생했습니다.</v>
+        <v>거래처 미팅이 있습니다.</v>
       </c>
       <c r="B27" t="str">
-        <v>A problem has occurred.</v>
+        <v>I have a meeting with a client.</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>해결 방안을 모색 중입니다.</v>
+        <v>견적서 보내주세요.</v>
       </c>
       <c r="B28" t="str">
-        <v>We are looking for a solution.</v>
+        <v>Please send me the quotation.</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>성공적으로 완료되었습니다.</v>
+        <v>계약이 성사되었습니다.</v>
       </c>
       <c r="B29" t="str">
-        <v>It has been successfully completed.</v>
+        <v>The contract has been signed.</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>실적 보고회가 있습니다.</v>
+        <v>프로젝트 진행 상황 보고해주세요.</v>
       </c>
       <c r="B30" t="str">
-        <v>There is a performance report meeting.</v>
+        <v>Please report the project progress.</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>야근을 해야 합니다.</v>
+        <v>수고하세요.</v>
       </c>
       <c r="B31" t="str">
-        <v>I have to work overtime.</v>
+        <v>Keep up the good work. (Formal greeting)</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>주말 근무는 없습니다.</v>
+        <v>자료 준비되었습니다.</v>
       </c>
       <c r="B32" t="str">
-        <v>There is no weekend work.</v>
+        <v>The materials are ready.</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>연차 휴가를 신청합니다.</v>
+        <v>언제 시간 되시나요?</v>
       </c>
       <c r="B33" t="str">
-        <v>I apply for annual leave.</v>
+        <v>When are you available?</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>병가를 냈습니다.</v>
+        <v>점심 식사 하셨습니까?</v>
       </c>
       <c r="B34" t="str">
-        <v>I took sick leave.</v>
+        <v>Have you had lunch?</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>조퇴하겠습니다.</v>
+        <v>커피 한 잔 하시겠습니까?</v>
       </c>
       <c r="B35" t="str">
-        <v>I will leave early.</v>
+        <v>Would you like a cup of coffee?</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>지각해서 죄송합니다.</v>
+        <v>잠시 자리 비우셨습니다.</v>
       </c>
       <c r="B36" t="str">
-        <v>I am sorry for being late.</v>
+        <v>He/She is away from the desk for a moment.</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>출근했습니다.</v>
+        <v>메모 남겨드릴까요?</v>
       </c>
       <c r="B37" t="str">
-        <v>I have arrived at work.</v>
+        <v>Shall I leave a message?</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>퇴근하겠습니다.</v>
+        <v>팩스로 보내주세요.</v>
       </c>
       <c r="B38" t="str">
-        <v>I am leaving work.</v>
+        <v>Please send it by fax.</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>점심 식사 맛있게 하세요.</v>
+        <v>프레젠테이션 준비 완료했습니다.</v>
       </c>
       <c r="B39" t="str">
-        <v>Enjoy your lunch.</v>
+        <v>Presentation preparation is complete.</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>오늘 회식 참석하시나요?</v>
+        <v>예산안 검토 부탁드립니다.</v>
       </c>
       <c r="B40" t="str">
-        <v>Are you attending the company dinner today?</v>
+        <v>Please review the budget proposal.</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>명함 좀 주시겠습니까?</v>
+        <v>다음 주 일정 잡겠습니다.</v>
       </c>
       <c r="B41" t="str">
-        <v>Could you give me your business card?</v>
+        <v>I will schedule it for next week.</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>제 명함입니다.</v>
+        <v>출근했습니다.</v>
       </c>
       <c r="B42" t="str">
-        <v>Here is my business card.</v>
+        <v>I have arrived at work.</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>소개해 드리겠습니다.</v>
+        <v>병가 내겠습니다.</v>
       </c>
       <c r="B43" t="str">
-        <v>Let me introduce you.</v>
+        <v>I will take a sick leave.</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>우리 팀장님입니다.</v>
+        <v>연차 쓰겠습니다.</v>
       </c>
       <c r="B44" t="str">
-        <v>This is our team leader.</v>
+        <v>I will use my annual leave.</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>신입 사원입니다.</v>
+        <v>급한 일입니까?</v>
       </c>
       <c r="B45" t="str">
-        <v>This is a new employee.</v>
+        <v>Is it urgent?</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>인수인계 중입니다.</v>
+        <v>우선순위가 어떻게 되나요?</v>
       </c>
       <c r="B46" t="str">
-        <v>I am in the middle of handover.</v>
+        <v>What is the priority?</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>업무 분장이 필요합니다.</v>
+        <v>피드백 부탁드립니다.</v>
       </c>
       <c r="B47" t="str">
-        <v>Division of duties is needed.</v>
+        <v>Please give me feedback.</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>효율성을 높여야 합니다.</v>
+        <v>수정해서 다시 보내겠습니다.</v>
       </c>
       <c r="B48" t="str">
-        <v>We need to increase efficiency.</v>
+        <v>I will revise and resend it.</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>비용을 절감해야 합니다.</v>
+        <v>성공적인 프로젝트였습니다.</v>
       </c>
       <c r="B49" t="str">
-        <v>We need to cut costs.</v>
+        <v>It was a successful project.</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>고객 만족도가 중요합니다.</v>
+        <v>함께 일해서 즐거웠습니다.</v>
       </c>
       <c r="B50" t="str">
-        <v>Customer satisfaction is important.</v>
+        <v>It was a pleasure working with you.</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>시장 조사를 했습니다.</v>
+        <v>앞으로도 잘 부탁드립니다.</v>
       </c>
       <c r="B51" t="str">
-        <v>We conducted market research.</v>
+        <v>I look forward to working with you.</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>경쟁사를 분석했습니다.</v>
+        <v>안녕하십니까.</v>
       </c>
       <c r="B52" t="str">
-        <v>We analyzed competitors.</v>
+        <v>Hello (formal).</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>전략을 세웠습니다.</v>
+        <v>처음 뵙겠습니다.</v>
       </c>
       <c r="B53" t="str">
-        <v>We established a strategy.</v>
+        <v>Nice to meet you (first time).</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>목표를 달성했습니다.</v>
+        <v>잘 부탁드립니다.</v>
       </c>
       <c r="B54" t="str">
-        <v>We achieved the goal.</v>
+        <v>I look forward to your cooperation.</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>성과급이 지급됩니다.</v>
+        <v>오랜만입니다.</v>
       </c>
       <c r="B55" t="str">
-        <v>Performance bonuses will be paid.</v>
+        <v>Long time no see (formal).</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>승진을 축하합니다.</v>
+        <v>그동안 잘 지내셨습니까?</v>
       </c>
       <c r="B56" t="str">
-        <v>Congratulations on your promotion.</v>
+        <v>How have you been (formal)?</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>퇴사하게 되었습니다.</v>
+        <v>소개해 드리겠습니다.</v>
       </c>
       <c r="B57" t="str">
-        <v>I am resigning.</v>
+        <v>Let me introduce you.</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>그동안 감사했습니다.</v>
+        <v>이쪽은 제 동료입니다.</v>
       </c>
       <c r="B58" t="str">
-        <v>Thank you for everything.</v>
+        <v>This is my colleague.</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>송별회가 있습니다.</v>
+        <v>명함 교환하시죠.</v>
       </c>
       <c r="B59" t="str">
-        <v>There is a farewell party.</v>
+        <v>Let's exchange business cards.</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>환영회가 있습니다.</v>
+        <v>연락처를 알 수 있을까요?</v>
       </c>
       <c r="B60" t="str">
-        <v>There is a welcome party.</v>
+        <v>May I have your contact information?</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>워크숍을 갑니다.</v>
+        <v>이메일 주소 알려주세요.</v>
       </c>
       <c r="B61" t="str">
-        <v>We are going to a workshop.</v>
+        <v>Please tell me the email address.</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>세미나에 참석합니다.</v>
+        <v>전화 연결해 드리겠습니다.</v>
       </c>
       <c r="B62" t="str">
-        <v>I am attending a seminar.</v>
+        <v>I'll connect you.</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>교육을 받습니다.</v>
+        <v>부재중입니다.</v>
       </c>
       <c r="B63" t="str">
-        <v>I am receiving training.</v>
+        <v>He/She is currently unavailable/out of office.</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>자격증을 취득했습니다.</v>
+        <v>나중에 다시 걸겠습니다.</v>
       </c>
       <c r="B64" t="str">
-        <v>I obtained a certification.</v>
+        <v>I'll call back later.</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>외국어 능력이 필요합니다.</v>
+        <v>메시지를 남기시겠습니까?</v>
       </c>
       <c r="B65" t="str">
-        <v>Foreign language skills are required.</v>
+        <v>Would you like to leave a message?</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>프레젠테이션을 잘했습니다.</v>
+        <v>잘 안 들립니다.</v>
       </c>
       <c r="B66" t="str">
-        <v>You did a good job on the presentation.</v>
+        <v>I can't hear you well.</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>질문 있습니까?</v>
+        <v>좀 더 크게 말씀해 주세요.</v>
       </c>
       <c r="B67" t="str">
-        <v>Do you have any questions?</v>
+        <v>Please speak up a little.</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>이해가 되시나요?</v>
+        <v>끊겠습니다.</v>
       </c>
       <c r="B68" t="str">
-        <v>Do you understand?</v>
+        <v>I'm hanging up.</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>다시 설명해 드리겠습니다.</v>
+        <v>회의실을 예약했습니다.</v>
       </c>
       <c r="B69" t="str">
-        <v>I will explain it again.</v>
+        <v>I reserved the meeting room.</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>요점을 정리해주세요.</v>
+        <v>빔 프로젝터가 필요합니다.</v>
       </c>
       <c r="B70" t="str">
-        <v>Please summarize the main points.</v>
+        <v>I need a beam projector.</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>회의록을 작성해주세요.</v>
+        <v>자료를 복사해 주세요.</v>
       </c>
       <c r="B71" t="str">
-        <v>Please write the meeting minutes.</v>
+        <v>Please copy the materials.</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>아이디어가 좋습니다.</v>
+        <v>회의록을 작성하겠습니다.</v>
       </c>
       <c r="B72" t="str">
-        <v>That's a good idea.</v>
+        <v>I will write the minutes.</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>다른 의견 있습니까?</v>
+        <v>안건이 무엇입니까?</v>
       </c>
       <c r="B73" t="str">
-        <v>Any other opinions?</v>
+        <v>What is the agenda?</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>만장일치로 통과되었습니다.</v>
+        <v>결론을 내립시다.</v>
       </c>
       <c r="B74" t="str">
-        <v>It was passed unanimously.</v>
+        <v>Let's come to a conclusion.</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>반대 의견이 있습니다.</v>
+        <v>다음 회의는 언제입니까?</v>
       </c>
       <c r="B75" t="str">
-        <v>There is a dissenting opinion.</v>
+        <v>When is the next meeting?</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>절충안을 찾읍시다.</v>
+        <v>참석해 주셔서 감사합니다.</v>
       </c>
       <c r="B76" t="str">
-        <v>Let's find a compromise.</v>
+        <v>Thank you for attending.</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>결론을 내립시다.</v>
+        <v>추가 질문 있습니까?</v>
       </c>
       <c r="B77" t="str">
-        <v>Let's draw a conclusion.</v>
+        <v>Any further questions?</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>다음 안건으로 넘어갑시다.</v>
+        <v>시간이 부족합니다.</v>
       </c>
       <c r="B78" t="str">
-        <v>Let's move on to the next item.</v>
+        <v>We are running out of time.</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>시간이 부족합니다.</v>
+        <v>잠시 쉬겠습니다.</v>
       </c>
       <c r="B79" t="str">
-        <v>We are running out of time.</v>
+        <v>Let's take a break.</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>잠시 쉬었다 합시다.</v>
+        <v>이만 마치겠습니다.</v>
       </c>
       <c r="B80" t="str">
-        <v>Let's take a short break.</v>
+        <v>We will wrap up now.</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>오늘 회의는 여기까지입니다.</v>
+        <v>보고서를 검토했습니다.</v>
       </c>
       <c r="B81" t="str">
-        <v>That's all for today's meeting.</v>
+        <v>I reviewed the report.</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>수고 많으셨습니다.</v>
+        <v>수정이 필요합니다.</v>
       </c>
       <c r="B82" t="str">
-        <v>Thank you for your hard work.</v>
+        <v>It needs revision.</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>좋은 주말 보내세요.</v>
+        <v>오타가 있습니다.</v>
       </c>
       <c r="B83" t="str">
-        <v>Have a good weekend.</v>
+        <v>There is a typo.</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>월요일에 뵙겠습니다.</v>
+        <v>내용이 부족합니다.</v>
       </c>
       <c r="B84" t="str">
-        <v>See you on Monday.</v>
+        <v>The content is insufficient.</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>복사가 안 됩니다.</v>
+        <v>다시 작성해 주세요.</v>
       </c>
       <c r="B85" t="str">
-        <v>The copier is not working.</v>
+        <v>Please rewrite it.</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>프린터 용지가 없습니다.</v>
+        <v>잘 작성되었습니다.</v>
       </c>
       <c r="B86" t="str">
-        <v>The printer is out of paper.</v>
+        <v>It is well written.</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>인터넷이 느립니다.</v>
+        <v>승인 받았습니다.</v>
       </c>
       <c r="B87" t="str">
-        <v>The internet is slow.</v>
+        <v>It has been approved.</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>서버가 다운되었습니다.</v>
+        <v>반려되었습니다.</v>
       </c>
       <c r="B88" t="str">
-        <v>The server is down.</v>
+        <v>It has been rejected.</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>보안이 중요합니다.</v>
+        <v>기한을 연장할 수 있나요?</v>
       </c>
       <c r="B89" t="str">
-        <v>Security is important.</v>
+        <v>Can we extend the deadline?</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>비밀번호를 변경하세요.</v>
+        <v>최대한 빨리 처리하겠습니다.</v>
       </c>
       <c r="B90" t="str">
-        <v>Please change your password.</v>
+        <v>I will process it as soon as possible.</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>로그인이 안 됩니다.</v>
+        <v>문제가 해결되었습니다.</v>
       </c>
       <c r="B91" t="str">
-        <v>I can't log in.</v>
+        <v>The problem has been resolved.</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>IT 팀에 문의하세요.</v>
+        <v>컴퓨터가 고장났습니다.</v>
       </c>
       <c r="B92" t="str">
-        <v>Please contact the IT team.</v>
+        <v>The computer is broken.</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>탕비실에 커피가 없습니다.</v>
+        <v>인터넷이 안 됩니다.</v>
       </c>
       <c r="B93" t="str">
-        <v>There is no coffee in the pantry.</v>
+        <v>The internet is not working.</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>에어컨이 너무 춥습니다.</v>
+        <v>비밀번호를 잊어버렸습니다.</v>
       </c>
       <c r="B94" t="str">
-        <v>The air conditioner is too cold.</v>
+        <v>I forgot my password.</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>히터 좀 틀어주세요.</v>
+        <v>로그인이 안 됩니다.</v>
       </c>
       <c r="B95" t="str">
-        <v>Please turn on the heater.</v>
+        <v>I can't log in.</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>창문 좀 열어주세요.</v>
+        <v>파일이 안 열립니다.</v>
       </c>
       <c r="B96" t="str">
-        <v>Please open the window.</v>
+        <v>The file won't open.</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>청소 업체 불라주세요.</v>
+        <v>바이러스에 감염되었습니다.</v>
       </c>
       <c r="B97" t="str">
-        <v>Please call the cleaning service.</v>
+        <v>It is infected with a virus.</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>택배가 도착했습니다.</v>
+        <v>백업을 해야 합니다.</v>
       </c>
       <c r="B98" t="str">
-        <v>A package has arrived.</v>
+        <v>We need to backup.</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>우편물 확인해주세요.</v>
+        <v>소프트웨어를 업데이트하세요.</v>
       </c>
       <c r="B99" t="str">
-        <v>Please check the mail.</v>
+        <v>Please update the software.</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>주차권 필요하세요?</v>
+        <v>재부팅해 보세요.</v>
       </c>
       <c r="B100" t="str">
-        <v>Do you need a parking ticket?</v>
+        <v>Try rebooting.</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>엘리베이터가 고장났습니다.</v>
+        <v>IT 지원팀에 연락하세요.</v>
       </c>
       <c r="B101" t="str">
-        <v>The elevator is broken.</v>
+        <v>Contact IT support.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add multilingual Excel resources for Japanese and Chinese speakers
</commit_message>
<xml_diff>
--- a/assets/files/samples/business_korean.xlsx
+++ b/assets/files/samples/business_korean.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -810,409 +810,9 @@
         <v>I look forward to working with you.</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>안녕하십니까.</v>
-      </c>
-      <c r="B52" t="str">
-        <v>Hello (formal).</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>처음 뵙겠습니다.</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Nice to meet you (first time).</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>잘 부탁드립니다.</v>
-      </c>
-      <c r="B54" t="str">
-        <v>I look forward to your cooperation.</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>오랜만입니다.</v>
-      </c>
-      <c r="B55" t="str">
-        <v>Long time no see (formal).</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>그동안 잘 지내셨습니까?</v>
-      </c>
-      <c r="B56" t="str">
-        <v>How have you been (formal)?</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>소개해 드리겠습니다.</v>
-      </c>
-      <c r="B57" t="str">
-        <v>Let me introduce you.</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>이쪽은 제 동료입니다.</v>
-      </c>
-      <c r="B58" t="str">
-        <v>This is my colleague.</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>명함 교환하시죠.</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Let's exchange business cards.</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>연락처를 알 수 있을까요?</v>
-      </c>
-      <c r="B60" t="str">
-        <v>May I have your contact information?</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="str">
-        <v>이메일 주소 알려주세요.</v>
-      </c>
-      <c r="B61" t="str">
-        <v>Please tell me the email address.</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="str">
-        <v>전화 연결해 드리겠습니다.</v>
-      </c>
-      <c r="B62" t="str">
-        <v>I'll connect you.</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="str">
-        <v>부재중입니다.</v>
-      </c>
-      <c r="B63" t="str">
-        <v>He/She is currently unavailable/out of office.</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>나중에 다시 걸겠습니다.</v>
-      </c>
-      <c r="B64" t="str">
-        <v>I'll call back later.</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>메시지를 남기시겠습니까?</v>
-      </c>
-      <c r="B65" t="str">
-        <v>Would you like to leave a message?</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>잘 안 들립니다.</v>
-      </c>
-      <c r="B66" t="str">
-        <v>I can't hear you well.</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>좀 더 크게 말씀해 주세요.</v>
-      </c>
-      <c r="B67" t="str">
-        <v>Please speak up a little.</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>끊겠습니다.</v>
-      </c>
-      <c r="B68" t="str">
-        <v>I'm hanging up.</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>회의실을 예약했습니다.</v>
-      </c>
-      <c r="B69" t="str">
-        <v>I reserved the meeting room.</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>빔 프로젝터가 필요합니다.</v>
-      </c>
-      <c r="B70" t="str">
-        <v>I need a beam projector.</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>자료를 복사해 주세요.</v>
-      </c>
-      <c r="B71" t="str">
-        <v>Please copy the materials.</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>회의록을 작성하겠습니다.</v>
-      </c>
-      <c r="B72" t="str">
-        <v>I will write the minutes.</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>안건이 무엇입니까?</v>
-      </c>
-      <c r="B73" t="str">
-        <v>What is the agenda?</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>결론을 내립시다.</v>
-      </c>
-      <c r="B74" t="str">
-        <v>Let's come to a conclusion.</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>다음 회의는 언제입니까?</v>
-      </c>
-      <c r="B75" t="str">
-        <v>When is the next meeting?</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>참석해 주셔서 감사합니다.</v>
-      </c>
-      <c r="B76" t="str">
-        <v>Thank you for attending.</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>추가 질문 있습니까?</v>
-      </c>
-      <c r="B77" t="str">
-        <v>Any further questions?</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>시간이 부족합니다.</v>
-      </c>
-      <c r="B78" t="str">
-        <v>We are running out of time.</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="str">
-        <v>잠시 쉬겠습니다.</v>
-      </c>
-      <c r="B79" t="str">
-        <v>Let's take a break.</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="str">
-        <v>이만 마치겠습니다.</v>
-      </c>
-      <c r="B80" t="str">
-        <v>We will wrap up now.</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="str">
-        <v>보고서를 검토했습니다.</v>
-      </c>
-      <c r="B81" t="str">
-        <v>I reviewed the report.</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="str">
-        <v>수정이 필요합니다.</v>
-      </c>
-      <c r="B82" t="str">
-        <v>It needs revision.</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="str">
-        <v>오타가 있습니다.</v>
-      </c>
-      <c r="B83" t="str">
-        <v>There is a typo.</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="str">
-        <v>내용이 부족합니다.</v>
-      </c>
-      <c r="B84" t="str">
-        <v>The content is insufficient.</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="str">
-        <v>다시 작성해 주세요.</v>
-      </c>
-      <c r="B85" t="str">
-        <v>Please rewrite it.</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>잘 작성되었습니다.</v>
-      </c>
-      <c r="B86" t="str">
-        <v>It is well written.</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="str">
-        <v>승인 받았습니다.</v>
-      </c>
-      <c r="B87" t="str">
-        <v>It has been approved.</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="str">
-        <v>반려되었습니다.</v>
-      </c>
-      <c r="B88" t="str">
-        <v>It has been rejected.</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="str">
-        <v>기한을 연장할 수 있나요?</v>
-      </c>
-      <c r="B89" t="str">
-        <v>Can we extend the deadline?</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="str">
-        <v>최대한 빨리 처리하겠습니다.</v>
-      </c>
-      <c r="B90" t="str">
-        <v>I will process it as soon as possible.</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="str">
-        <v>문제가 해결되었습니다.</v>
-      </c>
-      <c r="B91" t="str">
-        <v>The problem has been resolved.</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="str">
-        <v>컴퓨터가 고장났습니다.</v>
-      </c>
-      <c r="B92" t="str">
-        <v>The computer is broken.</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="str">
-        <v>인터넷이 안 됩니다.</v>
-      </c>
-      <c r="B93" t="str">
-        <v>The internet is not working.</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="str">
-        <v>비밀번호를 잊어버렸습니다.</v>
-      </c>
-      <c r="B94" t="str">
-        <v>I forgot my password.</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="str">
-        <v>로그인이 안 됩니다.</v>
-      </c>
-      <c r="B95" t="str">
-        <v>I can't log in.</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="str">
-        <v>파일이 안 열립니다.</v>
-      </c>
-      <c r="B96" t="str">
-        <v>The file won't open.</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="str">
-        <v>바이러스에 감염되었습니다.</v>
-      </c>
-      <c r="B97" t="str">
-        <v>It is infected with a virus.</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="str">
-        <v>백업을 해야 합니다.</v>
-      </c>
-      <c r="B98" t="str">
-        <v>We need to backup.</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="str">
-        <v>소프트웨어를 업데이트하세요.</v>
-      </c>
-      <c r="B99" t="str">
-        <v>Please update the software.</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="str">
-        <v>재부팅해 보세요.</v>
-      </c>
-      <c r="B100" t="str">
-        <v>Try rebooting.</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="str">
-        <v>IT 지원팀에 연락하세요.</v>
-      </c>
-      <c r="B101" t="str">
-        <v>Contact IT support.</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B101"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B51"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>